<commit_message>
- adjusted model in rmd - updated excel-list with functions
</commit_message>
<xml_diff>
--- a/r_function_list.xlsx
+++ b/r_function_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bodog\OneDrive - Hochschule Luzern\Eigene Dateien\01_Ausbildung\03_HSLU_MSc_IDS\01_Module\02_FS20_R Bootcamp\Assignment\rb_repo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malik\Documents\rb_repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="77" documentId="11_AD4DB114E441178AC67DF47DA613C9FC683EDF19" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3F48F833-CB01-4742-A381-7AD2F5DAF053}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC3B155B-F20B-426D-82CF-AC8FBC1ADA43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="200">
   <si>
     <t>Function</t>
   </si>
@@ -585,13 +585,499 @@
       </rPr>
       <t> of the first argument.</t>
     </r>
+  </si>
+  <si>
+    <t>qqnorm()</t>
+  </si>
+  <si>
+    <t>qqplot</t>
+  </si>
+  <si>
+    <t>is a generic function which produces a normal QQ plot of the y-values (by default)</t>
+  </si>
+  <si>
+    <t>qqline adds a line to a “theoretical”, by default normal, quantile-quantile plo</t>
+  </si>
+  <si>
+    <t>qqline()</t>
+  </si>
+  <si>
+    <t>group_by()</t>
+  </si>
+  <si>
+    <t>dplyr</t>
+  </si>
+  <si>
+    <t>takes an existing tbl and converts it into a grouped tbl where operations are performed "by group"</t>
+  </si>
+  <si>
+    <t>ungroup()</t>
+  </si>
+  <si>
+    <t>removes grouping</t>
+  </si>
+  <si>
+    <t>Generates a new dataframe which has one (or more) rows for each combination of grouping variables </t>
+  </si>
+  <si>
+    <t>summarise() (note: used for grouping)</t>
+  </si>
+  <si>
+    <t>scale_x_log10()</t>
+  </si>
+  <si>
+    <t>transforms / scales data in the x-axis into logarithmic values</t>
+  </si>
+  <si>
+    <t>scale_color_brewer()</t>
+  </si>
+  <si>
+    <t>The brewer scales provides sequential, diverging and qualitative colour schemes from ColorBrewer</t>
+  </si>
+  <si>
+    <t>facet_wrap()</t>
+  </si>
+  <si>
+    <t>wraps a 1d sequence of panels into 2d. </t>
+  </si>
+  <si>
+    <t>ggtitle()</t>
+  </si>
+  <si>
+    <t>Use to explain the main findings</t>
+  </si>
+  <si>
+    <t>generates a new plot</t>
+  </si>
+  <si>
+    <t>ggplot()</t>
+  </si>
+  <si>
+    <t>cbind()</t>
+  </si>
+  <si>
+    <t>Combine R Objects by Rows or Columns</t>
+  </si>
+  <si>
+    <t>Aids the eye in seeing patterns in the presence of overplotting</t>
+  </si>
+  <si>
+    <t>stat_smooth()</t>
+  </si>
+  <si>
+    <t>The point geom is used to make scatterplots.</t>
+  </si>
+  <si>
+    <t>geom_point()</t>
+  </si>
+  <si>
+    <t>connects observation in order of the variable on the x axis</t>
+  </si>
+  <si>
+    <t>geom_line()</t>
+  </si>
+  <si>
+    <t>methods()</t>
+  </si>
+  <si>
+    <t>List all available methods for a S3 and S4 generic function, or all methods for an S3 or S4 class.</t>
+  </si>
+  <si>
+    <t>generates data frames - collections of variables</t>
+  </si>
+  <si>
+    <t>length()</t>
+  </si>
+  <si>
+    <t>returns the length of a character-string</t>
+  </si>
+  <si>
+    <t>pnorm()</t>
+  </si>
+  <si>
+    <t>calculates normal distribution probability</t>
+  </si>
+  <si>
+    <t>sd()</t>
+  </si>
+  <si>
+    <t>computes standard deviation</t>
+  </si>
+  <si>
+    <t>sum()</t>
+  </si>
+  <si>
+    <t>returns the sum of all the values present in its arguments</t>
+  </si>
+  <si>
+    <t>head()</t>
+  </si>
+  <si>
+    <t>Returns the first or last parts of a vector, matrix, table, data frame or function</t>
+  </si>
+  <si>
+    <t>filter()</t>
+  </si>
+  <si>
+    <t>finds rows/cases where conditions are true</t>
+  </si>
+  <si>
+    <t>select()</t>
+  </si>
+  <si>
+    <t>keeps only the variables you mention</t>
+  </si>
+  <si>
+    <t>arrange()</t>
+  </si>
+  <si>
+    <t>arrange() order the rows of a data frame rows by the values of selected columns</t>
+  </si>
+  <si>
+    <t>top_n()</t>
+  </si>
+  <si>
+    <t>Select top n rows (by value)</t>
+  </si>
+  <si>
+    <t>mutate()</t>
+  </si>
+  <si>
+    <t>mutate() adds new variables and preserves existing ones</t>
+  </si>
+  <si>
+    <t>read.csv()</t>
+  </si>
+  <si>
+    <t>Reads a file in table format</t>
+  </si>
+  <si>
+    <t>Reads a file in CSV format</t>
+  </si>
+  <si>
+    <t>replace_na()</t>
+  </si>
+  <si>
+    <t>tidyr</t>
+  </si>
+  <si>
+    <t>Replace NAs with specified values</t>
+  </si>
+  <si>
+    <t>levels()</t>
+  </si>
+  <si>
+    <t>levels provides access to the levels attribute of a variable</t>
+  </si>
+  <si>
+    <t>class()</t>
+  </si>
+  <si>
+    <t>returns object class</t>
+  </si>
+  <si>
+    <t>list()</t>
+  </si>
+  <si>
+    <t>Functions to construct, coerce and check for both kinds of R lists.</t>
+  </si>
+  <si>
+    <t>replace()</t>
+  </si>
+  <si>
+    <t>eplace replaces the values in x with indices given in list by those given in values.</t>
+  </si>
+  <si>
+    <t>Count the Number of Characters</t>
+  </si>
+  <si>
+    <t>nchar()</t>
+  </si>
+  <si>
+    <t>c()</t>
+  </si>
+  <si>
+    <t>Combine Values into a Vector or List</t>
+  </si>
+  <si>
+    <t>substr()</t>
+  </si>
+  <si>
+    <t>Extract or replace substrings in a character vector</t>
+  </si>
+  <si>
+    <t>matches a pattern against an element and replaces it</t>
+  </si>
+  <si>
+    <t>grepl()  / grep()  / gsub()</t>
+  </si>
+  <si>
+    <t>boxplot()</t>
+  </si>
+  <si>
+    <t>Produce box-and-whisker plot(s) of the given (grouped) values.</t>
+  </si>
+  <si>
+    <t>str()</t>
+  </si>
+  <si>
+    <t>Compactly Display the Structure of an Arbitrary R Object</t>
+  </si>
+  <si>
+    <t>table()</t>
+  </si>
+  <si>
+    <t>uses the cross-classifying factors to build a contingency table of the counts at each combination of factor levels.</t>
+  </si>
+  <si>
+    <t>t.test()</t>
+  </si>
+  <si>
+    <t>Performs one and two sample t-tests on vectors of data</t>
+  </si>
+  <si>
+    <t>A matrix of scatterplots is produced</t>
+  </si>
+  <si>
+    <t>pairs()</t>
+  </si>
+  <si>
+    <t>update()</t>
+  </si>
+  <si>
+    <t>update and refit a modell call</t>
+  </si>
+  <si>
+    <t>anova()</t>
+  </si>
+  <si>
+    <t>Compute analysis of variance (or deviance) tables for one or more fitted model objects.</t>
+  </si>
+  <si>
+    <t>fitted()</t>
+  </si>
+  <si>
+    <t>Extract Model Fitted Values from objects</t>
+  </si>
+  <si>
+    <t>par()</t>
+  </si>
+  <si>
+    <t>used to set or query graphical parameters</t>
+  </si>
+  <si>
+    <t>na.omit()</t>
+  </si>
+  <si>
+    <t>removes rows with missing values in objects</t>
+  </si>
+  <si>
+    <t>nrow()</t>
+  </si>
+  <si>
+    <t>returns the number of rows present in x</t>
+  </si>
+  <si>
+    <t>apply()</t>
+  </si>
+  <si>
+    <t>returns a vector or array or list of values obtained by applying a function to margins of an array or matrix</t>
+  </si>
+  <si>
+    <t>is.na()</t>
+  </si>
+  <si>
+    <t>indicated  which elements are missing</t>
+  </si>
+  <si>
+    <t>adds straigt lines to a plot</t>
+  </si>
+  <si>
+    <t>abline()</t>
+  </si>
+  <si>
+    <t>text()</t>
+  </si>
+  <si>
+    <t>adds text to a plot</t>
+  </si>
+  <si>
+    <t>points()</t>
+  </si>
+  <si>
+    <t>adds points to a plot</t>
+  </si>
+  <si>
+    <t>dev.off()</t>
+  </si>
+  <si>
+    <t>grDevices</t>
+  </si>
+  <si>
+    <t>gets back to default values</t>
+  </si>
+  <si>
+    <t>pdf()</t>
+  </si>
+  <si>
+    <t>PDF Graphics Device</t>
+  </si>
+  <si>
+    <t>getwd()</t>
+  </si>
+  <si>
+    <t>get working directory</t>
+  </si>
+  <si>
+    <t>setwd()</t>
+  </si>
+  <si>
+    <t>set working directory</t>
+  </si>
+  <si>
+    <t>identify()</t>
+  </si>
+  <si>
+    <t>identifies points in a scatter plot</t>
+  </si>
+  <si>
+    <t>locator()</t>
+  </si>
+  <si>
+    <t>reads position of graphics cursor when mouse is pressed</t>
+  </si>
+  <si>
+    <t>xyplot()</t>
+  </si>
+  <si>
+    <t>lattice</t>
+  </si>
+  <si>
+    <t>generates a plot</t>
+  </si>
+  <si>
+    <t>sessionInfo()</t>
+  </si>
+  <si>
+    <t>collects info about current r session</t>
+  </si>
+  <si>
+    <t>find()</t>
+  </si>
+  <si>
+    <t>finds objects by name</t>
+  </si>
+  <si>
+    <t>install.packages()</t>
+  </si>
+  <si>
+    <t>installes packages from repositories by name</t>
+  </si>
+  <si>
+    <t>lmer()</t>
+  </si>
+  <si>
+    <t>lme4</t>
+  </si>
+  <si>
+    <t>fits linear mixed-effects models</t>
+  </si>
+  <si>
+    <t>fits a generalized additive model</t>
+  </si>
+  <si>
+    <t>help is the primary interface to the help systems</t>
+  </si>
+  <si>
+    <t>help()</t>
+  </si>
+  <si>
+    <t>.libsPaths()</t>
+  </si>
+  <si>
+    <t>gets/sets the library trees within which packages are looked for</t>
+  </si>
+  <si>
+    <t>aprospos()</t>
+  </si>
+  <si>
+    <t>Find Objects by (Partial) Name</t>
+  </si>
+  <si>
+    <t>nlevels()</t>
+  </si>
+  <si>
+    <t>Return the number of levels which its argument has.</t>
+  </si>
+  <si>
+    <t>matrix()</t>
+  </si>
+  <si>
+    <t>generates a matrix from the given set of values</t>
+  </si>
+  <si>
+    <t>Combines Objects by Rows or Columns</t>
+  </si>
+  <si>
+    <t>rbind() /cbind()</t>
+  </si>
+  <si>
+    <t>view()</t>
+  </si>
+  <si>
+    <t>Invoke a spreadsheet-style data viewer on a matrix-like R object.</t>
+  </si>
+  <si>
+    <t>colnames()</t>
+  </si>
+  <si>
+    <t>Retrieve or set the row or column names of a matrix-like object.</t>
+  </si>
+  <si>
+    <t>seq()</t>
+  </si>
+  <si>
+    <t>generates regular sequences</t>
+  </si>
+  <si>
+    <t>rep()</t>
+  </si>
+  <si>
+    <t>rep replicates the values in x</t>
+  </si>
+  <si>
+    <t>read.table()</t>
+  </si>
+  <si>
+    <t>dim()</t>
+  </si>
+  <si>
+    <t>returns the dimension of an object</t>
+  </si>
+  <si>
+    <t>min()</t>
+  </si>
+  <si>
+    <t>max()</t>
+  </si>
+  <si>
+    <t>range()</t>
+  </si>
+  <si>
+    <t>returns the maxima of the inputs given</t>
+  </si>
+  <si>
+    <t>returns the minima of the inputs given</t>
+  </si>
+  <si>
+    <t>returns a vector containing the minimum and maximum of all the given arguments</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -969,20 +1455,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="C77" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C89" sqref="C89"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="32.28515625" customWidth="1"/>
-    <col min="2" max="2" width="29.85546875" customWidth="1"/>
-    <col min="3" max="3" width="140.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.36328125" customWidth="1"/>
+    <col min="2" max="2" width="29.81640625" customWidth="1"/>
+    <col min="3" max="3" width="140.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -993,7 +1479,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1004,7 +1490,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1015,7 +1501,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1026,7 +1512,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1037,7 +1523,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1048,7 +1534,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1059,7 +1545,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1070,7 +1556,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1081,7 +1567,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1092,7 +1578,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1103,7 +1589,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1114,7 +1600,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1125,7 +1611,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1136,7 +1622,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1145,6 +1631,875 @@
       </c>
       <c r="C15" s="2" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>63</v>
+      </c>
+      <c r="B27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>65</v>
+      </c>
+      <c r="B28" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>68</v>
+      </c>
+      <c r="B30" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>71</v>
+      </c>
+      <c r="B32" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>73</v>
+      </c>
+      <c r="B33" t="s">
+        <v>20</v>
+      </c>
+      <c r="C33" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>75</v>
+      </c>
+      <c r="B34" t="s">
+        <v>20</v>
+      </c>
+      <c r="C34" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>77</v>
+      </c>
+      <c r="B35" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>79</v>
+      </c>
+      <c r="B36" t="s">
+        <v>23</v>
+      </c>
+      <c r="C36" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>81</v>
+      </c>
+      <c r="B37" t="s">
+        <v>44</v>
+      </c>
+      <c r="C37" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
+        <v>83</v>
+      </c>
+      <c r="B38" t="s">
+        <v>44</v>
+      </c>
+      <c r="C38" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
+        <v>85</v>
+      </c>
+      <c r="B39" t="s">
+        <v>44</v>
+      </c>
+      <c r="C39" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
+        <v>87</v>
+      </c>
+      <c r="B40" t="s">
+        <v>44</v>
+      </c>
+      <c r="C40" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" t="s">
+        <v>89</v>
+      </c>
+      <c r="B41" t="s">
+        <v>44</v>
+      </c>
+      <c r="C41" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" t="s">
+        <v>91</v>
+      </c>
+      <c r="B42" t="s">
+        <v>23</v>
+      </c>
+      <c r="C42" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" t="s">
+        <v>94</v>
+      </c>
+      <c r="B43" t="s">
+        <v>95</v>
+      </c>
+      <c r="C43" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" t="s">
+        <v>97</v>
+      </c>
+      <c r="B44" t="s">
+        <v>18</v>
+      </c>
+      <c r="C44" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" t="s">
+        <v>99</v>
+      </c>
+      <c r="B45" t="s">
+        <v>18</v>
+      </c>
+      <c r="C45" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" t="s">
+        <v>101</v>
+      </c>
+      <c r="B46" t="s">
+        <v>18</v>
+      </c>
+      <c r="C46" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" t="s">
+        <v>103</v>
+      </c>
+      <c r="B47" t="s">
+        <v>18</v>
+      </c>
+      <c r="C47" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" t="s">
+        <v>106</v>
+      </c>
+      <c r="B48" t="s">
+        <v>18</v>
+      </c>
+      <c r="C48" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" t="s">
+        <v>107</v>
+      </c>
+      <c r="B49" t="s">
+        <v>18</v>
+      </c>
+      <c r="C49" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" t="s">
+        <v>109</v>
+      </c>
+      <c r="B50" t="s">
+        <v>18</v>
+      </c>
+      <c r="C50" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" t="s">
+        <v>112</v>
+      </c>
+      <c r="B51" t="s">
+        <v>18</v>
+      </c>
+      <c r="C51" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" t="s">
+        <v>113</v>
+      </c>
+      <c r="B52" t="s">
+        <v>21</v>
+      </c>
+      <c r="C52" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" t="s">
+        <v>115</v>
+      </c>
+      <c r="B53" t="s">
+        <v>23</v>
+      </c>
+      <c r="C53" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" t="s">
+        <v>117</v>
+      </c>
+      <c r="B54" t="s">
+        <v>18</v>
+      </c>
+      <c r="C54" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" t="s">
+        <v>119</v>
+      </c>
+      <c r="B55" t="s">
+        <v>20</v>
+      </c>
+      <c r="C55" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" t="s">
+        <v>122</v>
+      </c>
+      <c r="B56" t="s">
+        <v>21</v>
+      </c>
+      <c r="C56" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" t="s">
+        <v>123</v>
+      </c>
+      <c r="B57" t="s">
+        <v>20</v>
+      </c>
+      <c r="C57" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" t="s">
+        <v>125</v>
+      </c>
+      <c r="B58" t="s">
+        <v>20</v>
+      </c>
+      <c r="C58" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" t="s">
+        <v>127</v>
+      </c>
+      <c r="B59" t="s">
+        <v>20</v>
+      </c>
+      <c r="C59" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" t="s">
+        <v>129</v>
+      </c>
+      <c r="B60" t="s">
+        <v>21</v>
+      </c>
+      <c r="C60" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" t="s">
+        <v>131</v>
+      </c>
+      <c r="B61" t="s">
+        <v>20</v>
+      </c>
+      <c r="C61" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" t="s">
+        <v>133</v>
+      </c>
+      <c r="B62" t="s">
+        <v>18</v>
+      </c>
+      <c r="C62" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" t="s">
+        <v>135</v>
+      </c>
+      <c r="B63" t="s">
+        <v>18</v>
+      </c>
+      <c r="C63" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" t="s">
+        <v>137</v>
+      </c>
+      <c r="B64" t="s">
+        <v>18</v>
+      </c>
+      <c r="C64" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" t="s">
+        <v>140</v>
+      </c>
+      <c r="B65" t="s">
+        <v>21</v>
+      </c>
+      <c r="C65" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" t="s">
+        <v>141</v>
+      </c>
+      <c r="B66" t="s">
+        <v>21</v>
+      </c>
+      <c r="C66" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" t="s">
+        <v>143</v>
+      </c>
+      <c r="B67" t="s">
+        <v>21</v>
+      </c>
+      <c r="C67" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" t="s">
+        <v>145</v>
+      </c>
+      <c r="B68" t="s">
+        <v>146</v>
+      </c>
+      <c r="C68" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" t="s">
+        <v>148</v>
+      </c>
+      <c r="B69" t="s">
+        <v>146</v>
+      </c>
+      <c r="C69" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" t="s">
+        <v>150</v>
+      </c>
+      <c r="B70" t="s">
+        <v>18</v>
+      </c>
+      <c r="C70" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" t="s">
+        <v>152</v>
+      </c>
+      <c r="B71" t="s">
+        <v>18</v>
+      </c>
+      <c r="C71" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" t="s">
+        <v>154</v>
+      </c>
+      <c r="B72" t="s">
+        <v>21</v>
+      </c>
+      <c r="C72" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" t="s">
+        <v>156</v>
+      </c>
+      <c r="B73" t="s">
+        <v>21</v>
+      </c>
+      <c r="C73" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" t="s">
+        <v>158</v>
+      </c>
+      <c r="B74" t="s">
+        <v>159</v>
+      </c>
+      <c r="C74" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" t="s">
+        <v>161</v>
+      </c>
+      <c r="B75" t="s">
+        <v>23</v>
+      </c>
+      <c r="C75" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" t="s">
+        <v>163</v>
+      </c>
+      <c r="B76" t="s">
+        <v>23</v>
+      </c>
+      <c r="C76" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" t="s">
+        <v>165</v>
+      </c>
+      <c r="B77" t="s">
+        <v>23</v>
+      </c>
+      <c r="C77" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" t="s">
+        <v>167</v>
+      </c>
+      <c r="B78" t="s">
+        <v>168</v>
+      </c>
+      <c r="C78" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" t="s">
+        <v>5</v>
+      </c>
+      <c r="B79" t="s">
+        <v>19</v>
+      </c>
+      <c r="C79" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" t="s">
+        <v>172</v>
+      </c>
+      <c r="B80" t="s">
+        <v>23</v>
+      </c>
+      <c r="C80" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" t="s">
+        <v>173</v>
+      </c>
+      <c r="B81" t="s">
+        <v>18</v>
+      </c>
+      <c r="C81" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" t="s">
+        <v>175</v>
+      </c>
+      <c r="B82" t="s">
+        <v>23</v>
+      </c>
+      <c r="C82" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" t="s">
+        <v>177</v>
+      </c>
+      <c r="B83" t="s">
+        <v>18</v>
+      </c>
+      <c r="C83" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" t="s">
+        <v>179</v>
+      </c>
+      <c r="B84" t="s">
+        <v>18</v>
+      </c>
+      <c r="C84" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" t="s">
+        <v>182</v>
+      </c>
+      <c r="B85" t="s">
+        <v>18</v>
+      </c>
+      <c r="C85" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" t="s">
+        <v>183</v>
+      </c>
+      <c r="B86" t="s">
+        <v>23</v>
+      </c>
+      <c r="C86" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" t="s">
+        <v>185</v>
+      </c>
+      <c r="B87" t="s">
+        <v>18</v>
+      </c>
+      <c r="C87" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" t="s">
+        <v>187</v>
+      </c>
+      <c r="B88" t="s">
+        <v>18</v>
+      </c>
+      <c r="C88" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" t="s">
+        <v>189</v>
+      </c>
+      <c r="B89" t="s">
+        <v>18</v>
+      </c>
+      <c r="C89" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" t="s">
+        <v>191</v>
+      </c>
+      <c r="B90" t="s">
+        <v>23</v>
+      </c>
+      <c r="C90" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" t="s">
+        <v>192</v>
+      </c>
+      <c r="B91" t="s">
+        <v>18</v>
+      </c>
+      <c r="C91" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" t="s">
+        <v>194</v>
+      </c>
+      <c r="B92" t="s">
+        <v>18</v>
+      </c>
+      <c r="C92" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" t="s">
+        <v>195</v>
+      </c>
+      <c r="B93" t="s">
+        <v>18</v>
+      </c>
+      <c r="C93" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" t="s">
+        <v>196</v>
+      </c>
+      <c r="B94" t="s">
+        <v>18</v>
+      </c>
+      <c r="C94" t="s">
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -1153,6 +2508,6 @@
     <hyperlink ref="C3" r:id="rId2" display="http://127.0.0.1:18073/help/library/stats/help/aov" xr:uid="{0A97E826-4356-4B5F-AC64-2A43672AE274}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>